<commit_message>
ändrat numrering och ägartabell
</commit_message>
<xml_diff>
--- a/Diagram/kund usecases.xlsx
+++ b/Diagram/kund usecases.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\tommy\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1570CA89-B1D8-4121-8F4A-D4673F451A0B}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{7B63E62E-40BF-4A24-A918-15061EAF4B3D}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="17256" windowHeight="5652" activeTab="1" xr2:uid="{5D7989B9-4628-4F72-A8A8-7230C0813551}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="Kund" sheetId="1" r:id="rId1"/>
     <sheet name="Ägare" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="179017"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -56,10 +56,6 @@
     <t>Kund väljer "visa meny"</t>
   </si>
   <si>
-    <t>2.1 Kunden väljer att lägga till produkt från menyn
-2.2 Produkten läggs till i varukorgen</t>
-  </si>
-  <si>
     <t>Välja produkt</t>
   </si>
   <si>
@@ -80,47 +76,24 @@
     <t>Kunden trycker på "ta bort" varan</t>
   </si>
   <si>
-    <t>9.1 Kunden väljer att ta bort varan
-9.2 Varan tas bort från varukorgen
-9.3 Varukorgen uppdateras
-9.4 Varukorgen visas på nytt</t>
-  </si>
-  <si>
     <t>Byt ut en produkt i varukorgen</t>
   </si>
   <si>
     <t>Kunden trycker på "ändra" produkt</t>
   </si>
   <si>
-    <t>10.1 Kunden väljer att ändra produkt
-10.2 Produkten tas bort från varukorgen
-10.3 Kunden tas till menyn för välj produkt</t>
-  </si>
-  <si>
     <t>Öka antal av en produkt i varukorgen</t>
   </si>
   <si>
     <t>Kunden trycker på "+" för produkten</t>
   </si>
   <si>
-    <t>11.1 Kunden väljer att öka antal
-11.2 Antalet produkter ökas
-11.3 Varukorgen uppdateras
-11.4 Varukorgen visas på nytt</t>
-  </si>
-  <si>
     <t>Kunden trycker på "-" för produkten</t>
   </si>
   <si>
     <t>Minska antal av en produkt i varukorgen</t>
   </si>
   <si>
-    <t>12.1 Kunden väljer att minska antal
-12.2 Antalet produkter minskas
-12.3 Varukorgen uppdateras
-12.4 Varukorgen visas på nytt</t>
-  </si>
-  <si>
     <t>Granska varukorgen</t>
   </si>
   <si>
@@ -139,17 +112,41 @@
     <t>"Lägg till produkt" väljs från menyn</t>
   </si>
   <si>
-    <t>* Admin sida finns
-* Ägaren inloggad
+    <t>* app för ägare finns installerad
 * produkten måste finnas skapad</t>
   </si>
   <si>
-    <t xml:space="preserve">1 Ägaren loggar in som admin
-2. Ägaren väljer "lägg till produkt" 
-3. Lista med tillgängliga produkter visas
-4. produkt väljs
-5. produkt läggs till på menyn
-</t>
+    <t>1. Ägaren väljer "lägg till produkt" 
+2. Lista med tillgängliga produkter visas
+3. produkt väljs
+4. produkt läggs till på menyn</t>
+  </si>
+  <si>
+    <t>1 Kunden väljer att lägga till produkt från menyn
+2 Produkten läggs till i varukorgen</t>
+  </si>
+  <si>
+    <t>1 Kunden väljer att minska antal
+2 Antalet produkter minskas
+3 Varukorgen uppdateras
+4 Varukorgen visas på nytt</t>
+  </si>
+  <si>
+    <t>1 Kunden väljer att ta bort varan
+2 Varan tas bort från varukorgen
+3 Varukorgen uppdateras
+4 Varukorgen visas på nytt</t>
+  </si>
+  <si>
+    <t>1 Kunden väljer att ändra produkt
+2 Produkten tas bort från varukorgen
+3 Kunden tas till menyn för välj produkt</t>
+  </si>
+  <si>
+    <t>1 Kunden väljer att öka antal
+2 Antalet produkter ökas
+3 Varukorgen uppdateras
+4 Varukorgen visas på nytt</t>
   </si>
 </sst>
 </file>
@@ -657,8 +654,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{51E6CB66-D299-406D-AF32-EC225AF777E1}">
   <dimension ref="A3:B51"/>
   <sheetViews>
-    <sheetView topLeftCell="A46" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4:B8"/>
+    <sheetView topLeftCell="A43" workbookViewId="0">
+      <selection activeCell="B52" sqref="B52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -736,7 +733,7 @@
         <v>4</v>
       </c>
       <c r="B14" s="8" t="s">
-        <v>9</v>
+        <v>29</v>
       </c>
     </row>
     <row r="15" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
@@ -745,7 +742,7 @@
         <v>0</v>
       </c>
       <c r="B16" s="10" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.3">
@@ -761,7 +758,7 @@
         <v>2</v>
       </c>
       <c r="B18" s="7" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.3">
@@ -769,7 +766,7 @@
         <v>3</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="20" spans="1:2" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
@@ -777,7 +774,7 @@
         <v>4</v>
       </c>
       <c r="B20" s="8" t="s">
-        <v>9</v>
+        <v>29</v>
       </c>
     </row>
     <row r="21" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
@@ -786,7 +783,7 @@
         <v>0</v>
       </c>
       <c r="B22" s="10" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.3">
@@ -802,7 +799,7 @@
         <v>2</v>
       </c>
       <c r="B24" s="7" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.3">
@@ -810,7 +807,7 @@
         <v>3</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
     </row>
     <row r="26" spans="1:2" ht="58.2" thickBot="1" x14ac:dyDescent="0.35">
@@ -818,7 +815,7 @@
         <v>4</v>
       </c>
       <c r="B26" s="8" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
     </row>
     <row r="28" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
@@ -827,7 +824,7 @@
         <v>0</v>
       </c>
       <c r="B29" s="10" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.3">
@@ -843,7 +840,7 @@
         <v>2</v>
       </c>
       <c r="B31" s="7" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.3">
@@ -851,7 +848,7 @@
         <v>3</v>
       </c>
       <c r="B32" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="33" spans="1:2" ht="58.2" thickBot="1" x14ac:dyDescent="0.35">
@@ -859,7 +856,7 @@
         <v>4</v>
       </c>
       <c r="B33" s="8" t="s">
-        <v>16</v>
+        <v>31</v>
       </c>
     </row>
     <row r="34" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
@@ -868,7 +865,7 @@
         <v>0</v>
       </c>
       <c r="B35" s="10" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.3">
@@ -884,7 +881,7 @@
         <v>2</v>
       </c>
       <c r="B37" s="7" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.3">
@@ -892,7 +889,7 @@
         <v>3</v>
       </c>
       <c r="B38" s="3" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="39" spans="1:2" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
@@ -900,7 +897,7 @@
         <v>4</v>
       </c>
       <c r="B39" s="8" t="s">
-        <v>19</v>
+        <v>32</v>
       </c>
     </row>
     <row r="40" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
@@ -909,7 +906,7 @@
         <v>0</v>
       </c>
       <c r="B41" s="10" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.3">
@@ -925,7 +922,7 @@
         <v>2</v>
       </c>
       <c r="B43" s="7" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.3">
@@ -933,7 +930,7 @@
         <v>3</v>
       </c>
       <c r="B44" s="3" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
     </row>
     <row r="45" spans="1:2" ht="58.2" thickBot="1" x14ac:dyDescent="0.35">
@@ -941,7 +938,7 @@
         <v>4</v>
       </c>
       <c r="B45" s="8" t="s">
-        <v>22</v>
+        <v>33</v>
       </c>
     </row>
     <row r="46" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
@@ -950,7 +947,7 @@
         <v>0</v>
       </c>
       <c r="B47" s="10" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.3">
@@ -966,7 +963,7 @@
         <v>2</v>
       </c>
       <c r="B49" s="7" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.3">
@@ -974,7 +971,7 @@
         <v>3</v>
       </c>
       <c r="B50" s="3" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
     </row>
     <row r="51" spans="1:2" ht="58.2" thickBot="1" x14ac:dyDescent="0.35">
@@ -982,7 +979,7 @@
         <v>4</v>
       </c>
       <c r="B51" s="8" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
     </row>
   </sheetData>
@@ -996,7 +993,7 @@
   <dimension ref="A2:B7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1011,7 +1008,7 @@
         <v>0</v>
       </c>
       <c r="B3" s="10" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
@@ -1019,15 +1016,15 @@
         <v>1</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>2</v>
       </c>
       <c r="B5" s="7" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
@@ -1035,15 +1032,15 @@
         <v>3</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" ht="87" thickBot="1" x14ac:dyDescent="0.35">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" ht="58.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A7" s="4" t="s">
         <v>4</v>
       </c>
       <c r="B7" s="8" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
     </row>
   </sheetData>

</xml_diff>